<commit_message>
Added employees, sales, shops and sales reports tables
</commit_message>
<xml_diff>
--- a/MobiStore/Data/Reports/Input/2016.10.17/MobiStore Mladost-2016.10.17-The first sale report.xlsx
+++ b/MobiStore/Data/Reports/Input/2016.10.17/MobiStore Mladost-2016.10.17-The first sale report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="MobiStore Mladost" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MobiStore Mladost'!$A$1:$J$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,25 +439,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -489,7 +489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -522,7 +522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>